<commit_message>
Logic change for Logged in User
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC02_Verify_MYACC.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC02_Verify_MYACC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\Kaman_ECTEST_Sanity\Input_files\Actual_testcases\Kaman\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77BA9F4F-A704-46CC-A452-2B5B7DE1FE63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CCB4CF-EBC3-423F-94CA-6D8B682190BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -608,7 +608,7 @@
   <dimension ref="A1:E25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C5" sqref="C5:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1208,9 +1208,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1411,19 +1414,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1448,9 +1447,10 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DOM Changes in ECTEST
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC02_Verify_MYACC.xlsx
+++ b/Input_files/Actual_testcases/Kaman/ECTEST/ALL_PAGES/END_TO_END/TC02_Verify_MYACC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\ECTEST\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18CCB4CF-EBC3-423F-94CA-6D8B682190BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08870F5-BB11-4B62-8BA5-482865471CC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="54">
   <si>
     <t>TestCase</t>
   </si>
@@ -123,9 +123,6 @@
     <t>Quick order</t>
   </si>
   <si>
-    <t>Storeroooms</t>
-  </si>
-  <si>
     <t>Accounts</t>
   </si>
   <si>
@@ -190,6 +187,12 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>QuickOrderMyacc</t>
+  </si>
+  <si>
+    <t>Storerooms</t>
   </si>
 </sst>
 </file>
@@ -607,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5:C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -639,7 +642,7 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>5</v>
@@ -659,7 +662,7 @@
         <v>12</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E3" s="4"/>
     </row>
@@ -672,7 +675,7 @@
         <v>13</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E4" s="3"/>
     </row>
@@ -685,7 +688,7 @@
         <v>14</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>14</v>
@@ -700,7 +703,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
@@ -715,14 +718,14 @@
         <v>16</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E7" s="3"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -737,7 +740,7 @@
         <v>18</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>18</v>
@@ -752,7 +755,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E10" s="3"/>
     </row>
@@ -765,7 +768,7 @@
         <v>20</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>20</v>
@@ -780,7 +783,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>21</v>
@@ -795,7 +798,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E13" s="3"/>
     </row>
@@ -808,7 +811,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>22</v>
@@ -823,7 +826,7 @@
         <v>23</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>23</v>
@@ -838,7 +841,7 @@
         <v>24</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>24</v>
@@ -853,7 +856,7 @@
         <v>25</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>25</v>
@@ -868,7 +871,7 @@
         <v>26</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>26</v>
@@ -883,7 +886,7 @@
         <v>27</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>27</v>
@@ -895,10 +898,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>28</v>
@@ -910,10 +913,10 @@
         <v>11</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>29</v>
@@ -925,13 +928,13 @@
         <v>11</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -940,13 +943,13 @@
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -955,13 +958,13 @@
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -970,10 +973,10 @@
         <v>17</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25" s="3"/>
     </row>
@@ -988,8 +991,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1011,7 +1014,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1019,7 +1022,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1027,7 +1030,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1059,7 +1062,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -1067,7 +1070,7 @@
         <v>23</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -1075,7 +1078,7 @@
         <v>24</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -1120,39 +1123,39 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3" t="b">
         <v>1</v>
@@ -1160,15 +1163,15 @@
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B22" s="3" t="b">
         <v>1</v>
@@ -1176,7 +1179,7 @@
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B23" s="3" t="b">
         <v>1</v>
@@ -1184,7 +1187,7 @@
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B24" s="3" t="b">
         <v>1</v>
@@ -1192,7 +1195,7 @@
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B25" s="3" t="b">
         <v>1</v>
@@ -1208,12 +1211,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1414,15 +1414,19 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1447,10 +1451,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>